<commit_message>
Infografía 2 y 3
Integrecion de algunos grafícos
</commit_message>
<xml_diff>
--- a/data/Datos 2da Infografía.xlsx
+++ b/data/Datos 2da Infografía.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eladiomontero\Documents\Grupo Inco\inco_micitt\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inco_micitt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="6660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo Investigacion" sheetId="1" r:id="rId1"/>
     <sheet name="Proyectos Area Cient 2014" sheetId="2" r:id="rId2"/>
     <sheet name="I+D con respecto a ACT" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tipo Investigacion'!$A$1:$C$21</definedName>
+  </definedNames>
+  <calcPr calcId="162913" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>Todas las áreas</t>
   </si>
@@ -85,9 +92,6 @@
     <t>Brasil</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
@@ -114,11 +118,20 @@
   <si>
     <t>América Latina y el Caribe</t>
   </si>
+  <si>
+    <t>Etiquetas de columna</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Suma de Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,13 +169,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,6 +193,541 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Carlos Alemán" refreshedDate="42817.435735763887" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C21" sheet="Tipo Investigacion"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="tipo de investigación" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Investigación básica"/>
+        <s v="Investigación Aplicada"/>
+        <s v="Investigación Experimental"/>
+        <s v="Sin especificar"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="232" maxValue="2218"/>
+    </cacheField>
+    <cacheField name="Año" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2010" maxValue="2014" count="5">
+        <n v="2014"/>
+        <n v="2013"/>
+        <n v="2012"/>
+        <n v="2011"/>
+        <n v="2010"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Carlos Alemán" refreshedDate="42817.441455092594" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="37">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C38" sheet="Proyectos Area Cient 2014"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Todas las áreas" numFmtId="0">
+      <sharedItems count="8">
+        <s v="Ciencias exactas y naturales"/>
+        <s v="Ingeniería y tecnología"/>
+        <s v="Ciencias médicas"/>
+        <s v="Ciencias agrícolas"/>
+        <s v="Ciencias sociales"/>
+        <s v="Humanidades"/>
+        <s v="Otras"/>
+        <s v="No desagregados"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Año" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2010" maxValue="2014" count="5">
+        <n v="2014"/>
+        <n v="2013"/>
+        <n v="2012"/>
+        <n v="2011"/>
+        <n v="2010"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="7" maxValue="1383"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="0"/>
+    <n v="1108"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1492"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="352"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="309"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="1195"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1566"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="371"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="232"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="1128"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2146"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="366"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="438"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="1149"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2218"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="653"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="592"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="1054"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1657"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="722"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="552"/>
+    <x v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="37">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="620"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="423"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="394"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="853"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="800"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="139"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="688"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="332"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="501"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="786"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="691"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="145"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="191"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="710"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="358"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1007"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1016"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="721"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="139"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="127"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="753"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="346"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1116"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1383"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="714"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="146"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="154"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="765"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="423"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="505"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="1281"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="695"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="168"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="148"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E1:J6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Total" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E1:J10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="6"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Total" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,15 +993,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -458,8 +1020,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -469,8 +1037,26 @@
       <c r="C2">
         <v>2014</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>2010</v>
+      </c>
+      <c r="G2">
+        <v>2011</v>
+      </c>
+      <c r="H2">
+        <v>2012</v>
+      </c>
+      <c r="I2">
+        <v>2013</v>
+      </c>
+      <c r="J2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -480,8 +1066,26 @@
       <c r="C3">
         <v>2014</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1657</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2218</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2146</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1566</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -491,8 +1095,26 @@
       <c r="C4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1054</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1149</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1128</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1195</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -502,8 +1124,26 @@
       <c r="C5">
         <v>2014</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4">
+        <v>722</v>
+      </c>
+      <c r="G5" s="4">
+        <v>653</v>
+      </c>
+      <c r="H5" s="4">
+        <v>366</v>
+      </c>
+      <c r="I5" s="4">
+        <v>371</v>
+      </c>
+      <c r="J5" s="4">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -513,8 +1153,26 @@
       <c r="C6">
         <v>2013</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4">
+        <v>552</v>
+      </c>
+      <c r="G6" s="4">
+        <v>592</v>
+      </c>
+      <c r="H6" s="4">
+        <v>438</v>
+      </c>
+      <c r="I6" s="4">
+        <v>232</v>
+      </c>
+      <c r="J6" s="4">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -525,7 +1183,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -535,8 +1193,32 @@
       <c r="C8">
         <v>2013</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="str">
+        <f>"{ name: '"&amp;E3&amp;"',  data: ["</f>
+        <v>{ name: 'Investigación Aplicada',  data: [</v>
+      </c>
+      <c r="F8" t="str">
+        <f>F3&amp;","</f>
+        <v>1657,</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" ref="G8:I8" si="0">G3&amp;","</f>
+        <v>2218,</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>2146,</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>1566,</v>
+      </c>
+      <c r="J8" t="str">
+        <f>J3&amp;"]},"</f>
+        <v>1492]},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -546,8 +1228,32 @@
       <c r="C9">
         <v>2013</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
+        <f t="shared" ref="E9:E11" si="1">"{ name: '"&amp;E4&amp;"',  data: ["</f>
+        <v>{ name: 'Investigación básica',  data: [</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ref="F9:I11" si="2">F4&amp;","</f>
+        <v>1054,</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>1149,</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>1128,</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>1195,</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ref="J9:J11" si="3">J4&amp;"]},"</f>
+        <v>1108]},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -557,8 +1263,32 @@
       <c r="C10">
         <v>2012</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'Investigación Experimental',  data: [</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>722,</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>653,</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>366,</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>371,</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>352]},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -568,8 +1298,32 @@
       <c r="C11">
         <v>2012</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'Sin especificar',  data: [</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>552,</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>592,</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>438,</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
+        <v>232,</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>309]},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -580,7 +1334,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -591,7 +1345,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -602,7 +1356,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -613,7 +1367,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -680,24 +1434,29 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -707,8 +1466,14 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -718,8 +1483,26 @@
       <c r="C2">
         <v>620</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>2010</v>
+      </c>
+      <c r="G2">
+        <v>2011</v>
+      </c>
+      <c r="H2">
+        <v>2012</v>
+      </c>
+      <c r="I2">
+        <v>2013</v>
+      </c>
+      <c r="J2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -729,8 +1512,26 @@
       <c r="C3">
         <v>423</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1281</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1383</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1016</v>
+      </c>
+      <c r="I3" s="4">
+        <v>786</v>
+      </c>
+      <c r="J3" s="4">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -740,8 +1541,26 @@
       <c r="C4">
         <v>394</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>765</v>
+      </c>
+      <c r="G4" s="4">
+        <v>753</v>
+      </c>
+      <c r="H4" s="4">
+        <v>710</v>
+      </c>
+      <c r="I4" s="4">
+        <v>688</v>
+      </c>
+      <c r="J4" s="4">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -751,8 +1570,26 @@
       <c r="C5">
         <v>853</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>505</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1116</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1007</v>
+      </c>
+      <c r="I5" s="4">
+        <v>501</v>
+      </c>
+      <c r="J5" s="4">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -762,8 +1599,26 @@
       <c r="C6">
         <v>800</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>695</v>
+      </c>
+      <c r="G6" s="4">
+        <v>714</v>
+      </c>
+      <c r="H6" s="4">
+        <v>721</v>
+      </c>
+      <c r="I6" s="4">
+        <v>691</v>
+      </c>
+      <c r="J6" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -773,8 +1628,26 @@
       <c r="C7">
         <v>139</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4">
+        <v>168</v>
+      </c>
+      <c r="G7" s="4">
+        <v>146</v>
+      </c>
+      <c r="H7" s="4">
+        <v>139</v>
+      </c>
+      <c r="I7" s="4">
+        <v>145</v>
+      </c>
+      <c r="J7" s="4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -784,8 +1657,26 @@
       <c r="C8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>423</v>
+      </c>
+      <c r="G8" s="4">
+        <v>346</v>
+      </c>
+      <c r="H8" s="4">
+        <v>358</v>
+      </c>
+      <c r="I8" s="4">
+        <v>332</v>
+      </c>
+      <c r="J8" s="4">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -795,8 +1686,26 @@
       <c r="C9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4">
+        <v>148</v>
+      </c>
+      <c r="G9" s="4">
+        <v>154</v>
+      </c>
+      <c r="H9" s="4">
+        <v>127</v>
+      </c>
+      <c r="I9" s="4">
+        <v>191</v>
+      </c>
+      <c r="J9" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -806,8 +1715,20 @@
       <c r="C10">
         <v>688</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
+        <v>30</v>
+      </c>
+      <c r="J10" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -818,7 +1739,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -828,8 +1749,32 @@
       <c r="C12">
         <v>501</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" t="str">
+        <f>"{ name: '"&amp;E3&amp;"',  data: ["</f>
+        <v>{ name: 'Ciencias agrícolas',  data: [</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" ref="F12:I18" si="0">IF( ISBLANK( F3)=TRUE,"null", F3&amp;",")</f>
+        <v>1281,</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>1383,</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>1016,</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>786,</v>
+      </c>
+      <c r="J12" t="str">
+        <f>J3&amp;"]},"</f>
+        <v>853]},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -839,8 +1784,32 @@
       <c r="C13">
         <v>786</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
+        <f t="shared" ref="E13:E18" si="1">"{ name: '"&amp;E4&amp;"',  data: ["</f>
+        <v>{ name: 'Ciencias exactas y naturales',  data: [</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>765,</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>753,</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>710,</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>688,</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ref="J13:J19" si="2">J4&amp;"]},"</f>
+        <v>620]},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -850,8 +1819,32 @@
       <c r="C14">
         <v>691</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'Ciencias médicas',  data: [</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>505,</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>1116,</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>1007,</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>501,</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="2"/>
+        <v>394]},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -861,8 +1854,32 @@
       <c r="C15">
         <v>145</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'Ciencias sociales',  data: [</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>695,</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>714,</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>721,</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>691,</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="2"/>
+        <v>800]},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -872,8 +1889,32 @@
       <c r="C16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'Humanidades',  data: [</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>168,</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>146,</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>139,</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>145,</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="2"/>
+        <v>139]},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -883,8 +1924,32 @@
       <c r="C17">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'Ingeniería y tecnología',  data: [</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>423,</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>346,</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>358,</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>332,</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="2"/>
+        <v>423]},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -894,8 +1959,32 @@
       <c r="C18">
         <v>710</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name: 'No desagregados',  data: [</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>148,</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>154,</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>127,</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>191,</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="2"/>
+        <v>7]},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -905,8 +1994,32 @@
       <c r="C19">
         <v>358</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <f>"{ name: '"&amp;E10&amp;"',  data: ["</f>
+        <v>{ name: 'Otras',  data: [</v>
+      </c>
+      <c r="F19" t="str">
+        <f>IF( ISBLANK( F10)=TRUE,"null,", F10&amp;",")</f>
+        <v>null,</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ref="G19:I19" si="3">IF( ISBLANK( G10)=TRUE,"null,", G10&amp;",")</f>
+        <v>null,</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>null,</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="3"/>
+        <v>30,</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="2"/>
+        <v>25]},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -917,7 +2030,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -928,7 +2041,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -939,7 +2052,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -950,7 +2063,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -961,7 +2074,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -972,7 +2085,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -983,7 +2096,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -994,7 +2107,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +2118,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +2129,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +2140,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +2151,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1122,15 +2235,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1225,13 +2339,11 @@
       <c r="I3" s="1">
         <v>0.74425452078879539</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>0.3709330188533243</v>
@@ -1263,7 +2375,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>0.32252042219529981</v>
@@ -1295,7 +2407,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>0.60342146189735613</v>
@@ -1327,7 +2439,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>0.57171497105102675</v>
@@ -1359,7 +2471,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>0.36953699697100828</v>
@@ -1385,17 +2497,13 @@
       <c r="I8" s="1">
         <v>0.21390778533635676</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>0.11205796595551813</v>
       </c>
@@ -1423,7 +2531,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1">
         <v>0.46746425444993844</v>
@@ -1455,11 +2563,9 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1">
         <v>0.6494716486807588</v>
       </c>
@@ -1487,7 +2593,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>0.61092201647436162</v>
@@ -1515,6 +2621,468 @@
       </c>
       <c r="J12" s="1">
         <v>0.67307695912204213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>"{ name:'"&amp;A2&amp;"' , color:'#404040', data:["</f>
+        <v>{ name:'Argentina' , color:'#404040', data:[</v>
+      </c>
+      <c r="B15" t="str">
+        <f>IF(ISBLANK(B2)=TRUE,"null,", ROUND( B2,2)*100)&amp;","</f>
+        <v>86,</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" ref="C15:J15" si="0">IF(ISBLANK(C2)=TRUE,"null,", ROUND( C2,2)*100)&amp;","</f>
+        <v>84,</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>86,</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>93,</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>92,</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>92,</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>94,</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>94,</v>
+      </c>
+      <c r="J15" t="str">
+        <f>IF(ISBLANK(J2)=TRUE,"null,", ROUND( J2,2)*100)&amp;"]},"</f>
+        <v>92]},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" ref="A16:A25" si="1">"{ name:'"&amp;A3&amp;"' , color:'#404040', data:["</f>
+        <v>{ name:'Brasil' , color:'#404040', data:[</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" ref="B16:J25" si="2">IF(ISBLANK(B3)=TRUE,"null,", ROUND( B3,2)*100)&amp;","</f>
+        <v>78,</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="2"/>
+        <v>79,</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>77,</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>73,</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>72,</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>73,</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>71,</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v>74,</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ref="J16:J25" si="3">IF(ISBLANK(J3)=TRUE,"null,", ROUND( J3,2)*100)&amp;"]},"</f>
+        <v>null,]},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'Colombia' , color:'#404040', data:[</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="2"/>
+        <v>37,</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>39,</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>39,</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>42,</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>40,</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>42,</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>41,</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v>44,</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>39]},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'Costa Rica' , color:'#404040', data:[</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="2"/>
+        <v>32,</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v>27,</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>29,</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>28,</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>26,</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>27,</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>29,</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>28,</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>22]},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'Cuba' , color:'#404040', data:[</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>70,</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>60,</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>60]},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'México' , color:'#404040', data:[</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="2"/>
+        <v>57,</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="2"/>
+        <v>67,</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>68,</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>68,</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>72,</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>70,</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>67,</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v>67,</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>62]},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'Panamá' , color:'#404040', data:[</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="2"/>
+        <v>37,</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="2"/>
+        <v>39,</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>41,</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>35,</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>36,</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>38,</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>30,</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="2"/>
+        <v>21,</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="3"/>
+        <v>null,]},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'El Salvador' , color:'#404040', data:[</v>
+      </c>
+      <c r="B22" t="str">
+        <f>IF(ISBLANK(B9)=TRUE,"null,", ROUND( B9,2)*100)&amp;","</f>
+        <v>null,,</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" ref="C22:J22" si="4">IF(ISBLANK(C9)=TRUE,"null,", ROUND( C9,2)*100)&amp;","</f>
+        <v>11,</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="4"/>
+        <v>12,</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="4"/>
+        <v>8,</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="4"/>
+        <v>7,</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="4"/>
+        <v>3,</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="4"/>
+        <v>3,</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="4"/>
+        <v>5,</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>8]},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'Trinidad y Tobago' , color:'#404040', data:[</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="2"/>
+        <v>47,</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="2"/>
+        <v>45,</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>39,</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>36,</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>40,</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>36,</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>38,</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="2"/>
+        <v>41,</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="3"/>
+        <v>42]},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'Uruguay' , color:'#404040', data:[</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="2"/>
+        <v>null,,</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="2"/>
+        <v>65,</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>61,</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>59,</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>51,</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>59,</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>61,</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="2"/>
+        <v>62,</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="3"/>
+        <v>62]},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="1"/>
+        <v>{ name:'América Latina y el Caribe' , color:'#404040', data:[</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="2"/>
+        <v>61,</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="2"/>
+        <v>61,</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>61,</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>61,</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>64,</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>67,</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>65,</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="2"/>
+        <v>68,</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>67]},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>